<commit_message>
Add convolution multiprocessing. Not success
</commit_message>
<xml_diff>
--- a/test/resultsData/Результаты.xlsx
+++ b/test/resultsData/Результаты.xlsx
@@ -1,30 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PYTHON\Programms\ImageProcessingHandmade\test\resultsData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3398AA-BD0B-49C2-BC7F-BBE8AAC97B95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26205" windowHeight="11265"/>
+    <workbookView xWindow="15948" yWindow="552" windowWidth="13704" windowHeight="10296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>До</t>
   </si>
@@ -54,12 +60,21 @@
   </si>
   <si>
     <t>Общее (2 итерации)</t>
+  </si>
+  <si>
+    <t>16 ядер</t>
+  </si>
+  <si>
+    <t>convolutionConcurrentNN</t>
+  </si>
+  <si>
+    <t>42 значения</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -371,25 +386,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -399,10 +417,22 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
       </c>
       <c r="C3">
         <v>3.9</v>
@@ -414,8 +444,18 @@
         <f>C3/D3</f>
         <v>2.3076923076923079</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>12.1088</v>
+      </c>
+      <c r="G3">
+        <v>1.96376</v>
+      </c>
+      <c r="H3">
+        <f>F3/G3</f>
+        <v>6.1661302806860316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -429,8 +469,18 @@
         <f>C4/D4</f>
         <v>2.9662027924152246</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>14.848697</v>
+      </c>
+      <c r="G4">
+        <v>4.9652500000000002</v>
+      </c>
+      <c r="H4">
+        <f>F4/G4</f>
+        <v>2.9905235385932225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -440,21 +490,66 @@
       <c r="C5">
         <v>1.7230000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>0.82169999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6">
         <v>0.51200000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>0.31580000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7">
         <v>0.34300000000000003</v>
+      </c>
+      <c r="F7">
+        <v>9.4369999999999996E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>1.7230000000000001</v>
+      </c>
+      <c r="F9">
+        <v>17.101800000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="F10">
+        <v>0.31180000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="F11">
+        <v>8.2147000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add many test in convolution, results with multiprocessing good
</commit_message>
<xml_diff>
--- a/test/resultsData/Результаты.xlsx
+++ b/test/resultsData/Результаты.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PYTHON\Programms\ImageProcessingHandmade\test\resultsData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3398AA-BD0B-49C2-BC7F-BBE8AAC97B95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15E4BCA-A0F7-437C-A465-A1B61E2A5785}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15948" yWindow="552" windowWidth="13704" windowHeight="10296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13416" yWindow="600" windowWidth="13704" windowHeight="10296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -390,7 +390,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,7 +491,7 @@
         <v>1.7230000000000001</v>
       </c>
       <c r="F5">
-        <v>0.82169999999999999</v>
+        <v>18.975380000000001</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -506,6 +506,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>10000</v>
+      </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -513,7 +516,7 @@
         <v>0.34300000000000003</v>
       </c>
       <c r="F7">
-        <v>9.4369999999999996E-2</v>
+        <v>9.1827000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -527,7 +530,7 @@
         <v>1.7230000000000001</v>
       </c>
       <c r="F9">
-        <v>17.101800000000001</v>
+        <v>21.533545</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -542,6 +545,9 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10000</v>
+      </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -549,7 +555,7 @@
         <v>0.34300000000000003</v>
       </c>
       <c r="F11">
-        <v>8.2147000000000006</v>
+        <v>10.564019999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>